<commit_message>
FunctionFlow alias in not anymore mandatory Adapt excel import
</commit_message>
<xml_diff>
--- a/src/test/resources/junit/02-import-flows-02.xlsx
+++ b/src/test/resources/junit/02-import-flows-02.xlsx
@@ -197,7 +197,7 @@
     <t xml:space="preserve">EXT.001</t>
   </si>
   <si>
-    <t xml:space="preserve">S.02</t>
+    <t xml:space="preserve">CYP.02</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -474,7 +474,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.12"/>
   </cols>
@@ -618,10 +618,10 @@
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.59"/>

</xml_diff>